<commit_message>
test app and the test steps in excel file was updated
</commit_message>
<xml_diff>
--- a/doc/test_case_text_to_voice.xlsx
+++ b/doc/test_case_text_to_voice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91843\RWTV\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE5A3B-864F-4E6D-87BD-86BBA61CBF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9669B7FE-A9CC-4E6C-B4F7-CEAD7C872A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,57 +94,6 @@
     <t>Check exception handling</t>
   </si>
   <si>
-    <t>Check if the function is named 'text_to_speech()'</t>
-  </si>
-  <si>
-    <t>Provide different text inputs and verify processing</t>
-  </si>
-  <si>
-    <t>Provide an empty string and check response</t>
-  </si>
-  <si>
-    <t>Provide long text input and check if audio is generated</t>
-  </si>
-  <si>
-    <t>Provide text with special characters and verify correctness</t>
-  </si>
-  <si>
-    <t>Check if output can be saved in MP3 format</t>
-  </si>
-  <si>
-    <t>Check if output can be saved in WAV format</t>
-  </si>
-  <si>
-    <t>Verify if the generated speech can be encoded to Base64</t>
-  </si>
-  <si>
-    <t>Decode Base64 and check if the output matches original audio</t>
-  </si>
-  <si>
-    <t>Play the generated audio and verify clarity</t>
-  </si>
-  <si>
-    <t>Ensure response contains 'status' and 'audio' fields</t>
-  </si>
-  <si>
-    <t>Provide input in different languages and check response</t>
-  </si>
-  <si>
-    <t>Pass invalid inputs (numbers, symbols, null) and check handling</t>
-  </si>
-  <si>
-    <t>Ensure punctuation is maintained in speech</t>
-  </si>
-  <si>
-    <t>Measure time taken for long text conversion</t>
-  </si>
-  <si>
-    <t>Check if logs record process details</t>
-  </si>
-  <si>
-    <t>Verify proper handling of unexpected errors</t>
-  </si>
-  <si>
     <t>Function should be named 'text_to_speech()'</t>
   </si>
   <si>
@@ -359,6 +308,106 @@
   </si>
   <si>
     <t>RWS_TTV_00017</t>
+  </si>
+  <si>
+    <t>Step 1: Open test_text_to_speech.py.
+Step 2: Check if the function responsible for text-to-speech conversion is named text_to_speech().</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Provide different text inputs like:
+"Hello, how are you?"
+"This is a test of the TTS system."
+"Welcome to the AI voice assistant."</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Provide an empty string ("") as input.</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Provide a long paragraph as input. Example: "This is a long paragraph to test the capability of handling large text inputs...".</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Provide text with special characters, such as "Hello! How’s it going? @#$%^&amp;*()".</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Verify that the output is saved as MP3.</t>
+  </si>
+  <si>
+    <t>Step 1: Modify the function to export the generated audio as a WAV file.
+Step 2: Run the function and verify that a WAV file is created.</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Convert text to speech and verify if the output audio is encoded in Base64 format.</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Take the Base64 output, decode it, and verify if the original audio is restored.</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Provide input text and play the generated speech.</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Verify the response format of the function (check JSON structure).</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Provide inputs in different languages, such as "Hola, cómo estás?" (Spanish) or "Bonjour, comment ça va?" (French).</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Provide invalid inputs such as 12345, null, and symbols (#@&amp;%^).</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Provide a sentence with punctuation, such as "Hello, world! How's it going?".</t>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Provide a long text input and measure the time taken to generate speech.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Step 1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Check if the function logs process details such as input text, errors, and processing steps.</t>
+    </r>
+  </si>
+  <si>
+    <t>Step 1: Run test_text_to_speech.py.
+Step 2: Introduce errors (e.g., disconnect internet for online TTS, pass an invalid language code).</t>
   </si>
 </sst>
 </file>
@@ -434,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -442,11 +491,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -490,17 +567,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60206018-EB1A-48B7-B7A3-51E46BE324C7}" name="Table1" displayName="Table1" ref="A1:H18" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60206018-EB1A-48B7-B7A3-51E46BE324C7}" name="Table1" displayName="Table1" ref="A1:H18" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:H18" xr:uid="{60206018-EB1A-48B7-B7A3-51E46BE324C7}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{211A1D55-15D9-416E-8531-D4F10C345E0E}" name="Requirement ID"/>
-    <tableColumn id="2" xr3:uid="{FF4BA48F-5EB0-4F8B-89C1-CB7AB4DD99AF}" name="Testcase ID"/>
-    <tableColumn id="3" xr3:uid="{AF07C60F-A18C-4790-AAD8-CBBE59F6E7A7}" name="Test Case"/>
+    <tableColumn id="1" xr3:uid="{211A1D55-15D9-416E-8531-D4F10C345E0E}" name="Requirement ID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{FF4BA48F-5EB0-4F8B-89C1-CB7AB4DD99AF}" name="Testcase ID" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{AF07C60F-A18C-4790-AAD8-CBBE59F6E7A7}" name="Test Case" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{E61A431B-A797-4170-B710-E5E2BFC7FC25}" name="Test Steps"/>
-    <tableColumn id="5" xr3:uid="{95D2542B-54C9-4326-B93B-24E51ABED90F}" name="Expected Output"/>
-    <tableColumn id="6" xr3:uid="{9E69506F-0A16-43BB-8CA9-9AACEF31B753}" name="Actual Output"/>
-    <tableColumn id="7" xr3:uid="{75935E01-1BBB-4952-9BC1-B435368ADD7B}" name="Status"/>
-    <tableColumn id="8" xr3:uid="{E3654BBD-3196-4519-8581-8E4D15889F2E}" name="Comments"/>
+    <tableColumn id="5" xr3:uid="{95D2542B-54C9-4326-B93B-24E51ABED90F}" name="Expected Output" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{9E69506F-0A16-43BB-8CA9-9AACEF31B753}" name="Actual Output" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{75935E01-1BBB-4952-9BC1-B435368ADD7B}" name="Status" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{E3654BBD-3196-4519-8581-8E4D15889F2E}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -795,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,399 +910,416 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" t="s">
-        <v>67</v>
-      </c>
-      <c r="G11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>110</v>
-      </c>
-      <c r="B16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>111</v>
-      </c>
-      <c r="B17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="C18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F18" t="s">
-        <v>74</v>
-      </c>
-      <c r="G18" t="s">
-        <v>75</v>
-      </c>
+      <c r="G18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>